<commit_message>
Keeping vignette function table in sync with code
</commit_message>
<xml_diff>
--- a/vignettes/table_of_functions.xlsx
+++ b/vignettes/table_of_functions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="303">
   <si>
     <t>color.dendrogram</t>
   </si>
@@ -934,6 +934,9 @@
   </si>
   <si>
     <t>**find.local.minima**</t>
+  </si>
+  <si>
+    <t>deriv1.kde</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1717,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1987,7 +1990,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="6" t="s">
-        <v>158</v>
+        <v>302</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>263</v>

</xml_diff>

<commit_message>
added function to the summary table
</commit_message>
<xml_diff>
--- a/vignettes/table_of_functions.xlsx
+++ b/vignettes/table_of_functions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="305">
   <si>
     <t>color.dendrogram</t>
   </si>
@@ -937,6 +937,12 @@
   </si>
   <si>
     <t>deriv1.kde</t>
+  </si>
+  <si>
+    <t>ticklabels</t>
+  </si>
+  <si>
+    <t>Label powers of 10 tickmarks</t>
   </si>
 </sst>
 </file>
@@ -1714,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1871,163 +1877,171 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="6" t="s">
+      <c r="B17" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="B18" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="B19" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" s="6" t="s">
-        <v>191</v>
+        <v>300</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="B21" s="6" t="s">
-        <v>254</v>
+        <v>191</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="B25" s="6" t="s">
-        <v>152</v>
+        <v>301</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="B26" s="6" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" s="6" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="6" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" s="6" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="6" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="6" t="s">
-        <v>302</v>
+        <v>121</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="B32" s="6" t="s">
-        <v>253</v>
+        <v>302</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="B33" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="B34" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="6" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="B35" s="6" t="s">
+    <row r="36" spans="1:3">
+      <c r="B36" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>283</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing func name in table
</commit_message>
<xml_diff>
--- a/vignettes/table_of_functions.xlsx
+++ b/vignettes/table_of_functions.xlsx
@@ -939,10 +939,10 @@
     <t>deriv1.kde</t>
   </si>
   <si>
-    <t>ticklabels</t>
-  </si>
-  <si>
     <t>Label powers of 10 tickmarks</t>
+  </si>
+  <si>
+    <t>tick.labels</t>
   </si>
 </sst>
 </file>
@@ -1723,7 +1723,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1878,10 +1878,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="B17" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>303</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:3">

</xml_diff>

<commit_message>
updated function list to include ggflow
</commit_message>
<xml_diff>
--- a/vignettes/table_of_functions.xlsx
+++ b/vignettes/table_of_functions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogers/git/R/packages/wadeTools/vignettes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B475E8-C1B0-D84D-BEEF-235E6A053857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27360" yWindow="3280" windowWidth="23000" windowHeight="18800" tabRatio="879" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="879" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classutils" sheetId="1" r:id="rId1"/>
@@ -18,7 +24,7 @@
     <sheet name="ineractutils" sheetId="9" r:id="rId9"/>
     <sheet name="table_of_functions.csv" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="307">
   <si>
     <t>color.dendrogram</t>
   </si>
@@ -867,9 +873,6 @@
     <t>Calculate a Blob's Convexity</t>
   </si>
   <si>
-    <t>Draw a FlowJo-style (sort of) Plot</t>
-  </si>
-  <si>
     <t>Get the Gaussian Parameters of a GDE</t>
   </si>
   <si>
@@ -943,12 +946,21 @@
   </si>
   <si>
     <t>tick.labels</t>
+  </si>
+  <si>
+    <t>**ggflow**</t>
+  </si>
+  <si>
+    <t>Draw a FlowJo-style (sort of) Plot (DEPRECATED)</t>
+  </si>
+  <si>
+    <t>Draw a FlowJo-style (sort of) Plot (much more powerful version of pplot)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1211,6 +1223,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1535,21 +1555,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1560,12 +1580,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +1596,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1587,12 +1607,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1603,7 +1623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1611,7 +1631,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1619,7 +1639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1630,7 +1650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1641,7 +1661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1663,7 +1683,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -1674,7 +1694,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1685,7 +1705,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1696,7 +1716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -1719,21 +1739,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="20" style="6" customWidth="1"/>
     <col min="3" max="3" width="58.83203125" style="6" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>243</v>
       </c>
@@ -1744,18 +1764,18 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>291</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>110</v>
       </c>
@@ -1763,7 +1783,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>107</v>
       </c>
@@ -1771,7 +1791,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
@@ -1779,9 +1799,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>45</v>
@@ -1790,7 +1810,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>48</v>
       </c>
@@ -1798,34 +1818,34 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>247</v>
       </c>
@@ -1833,7 +1853,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>252</v>
       </c>
@@ -1841,7 +1861,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>249</v>
       </c>
@@ -1849,7 +1869,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>251</v>
       </c>
@@ -1857,192 +1877,200 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C19" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="B16" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="B18" s="6" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="B23" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="B25" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="B26" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="B27" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="B28" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="B29" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="B30" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="B31" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="B32" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="B33" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="B34" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="B35" s="6" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>282</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="B36" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -2057,14 +2085,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -2072,7 +2100,7 @@
     <col min="4" max="4" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2083,12 +2111,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>34</v>
       </c>
@@ -2096,7 +2124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>36</v>
       </c>
@@ -2107,7 +2135,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>39</v>
       </c>
@@ -2118,7 +2146,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -2141,14 +2169,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -2156,7 +2184,7 @@
     <col min="4" max="4" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2167,12 +2195,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>45</v>
       </c>
@@ -2183,12 +2211,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>48</v>
       </c>
@@ -2199,7 +2227,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>51</v>
       </c>
@@ -2207,7 +2235,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>53</v>
       </c>
@@ -2215,7 +2243,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>55</v>
       </c>
@@ -2226,7 +2254,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>58</v>
       </c>
@@ -2234,12 +2262,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>63</v>
       </c>
@@ -2262,14 +2290,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -2277,7 +2305,7 @@
     <col min="4" max="4" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2288,12 +2316,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -2316,14 +2344,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -2331,7 +2359,7 @@
     <col min="4" max="4" width="59.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2342,12 +2370,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60">
+    <row r="3" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>73</v>
       </c>
@@ -2358,12 +2386,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>78</v>
       </c>
@@ -2374,7 +2402,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>81</v>
       </c>
@@ -2385,7 +2413,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>84</v>
       </c>
@@ -2396,7 +2424,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>87</v>
       </c>
@@ -2407,7 +2435,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>89</v>
       </c>
@@ -2418,7 +2446,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>92</v>
       </c>
@@ -2429,7 +2457,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>95</v>
       </c>
@@ -2440,7 +2468,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>98</v>
       </c>
@@ -2451,7 +2479,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>101</v>
       </c>
@@ -2462,7 +2490,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45">
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>104</v>
       </c>
@@ -2473,12 +2501,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30">
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>107</v>
       </c>
@@ -2489,7 +2517,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>110</v>
       </c>
@@ -2500,12 +2528,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
+    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>114</v>
       </c>
@@ -2516,12 +2544,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>118</v>
       </c>
@@ -2532,7 +2560,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>121</v>
       </c>
@@ -2543,7 +2571,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>124</v>
       </c>
@@ -2554,7 +2582,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>127</v>
       </c>
@@ -2565,7 +2593,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>130</v>
       </c>
@@ -2576,7 +2604,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>133</v>
       </c>
@@ -2587,7 +2615,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30">
+    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>136</v>
       </c>
@@ -2598,7 +2626,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>139</v>
       </c>
@@ -2609,12 +2637,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>143</v>
       </c>
@@ -2625,7 +2653,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>146</v>
       </c>
@@ -2636,7 +2664,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>149</v>
       </c>
@@ -2647,7 +2675,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>152</v>
       </c>
@@ -2658,7 +2686,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>155</v>
       </c>
@@ -2669,7 +2697,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>158</v>
       </c>
@@ -2680,7 +2708,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>161</v>
       </c>
@@ -2691,12 +2719,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="60">
+    <row r="44" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>164</v>
       </c>
@@ -2707,7 +2735,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30">
+    <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>167</v>
       </c>
@@ -2718,7 +2746,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>84</v>
       </c>
@@ -2729,12 +2757,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30">
+    <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
         <v>173</v>
       </c>
@@ -2745,7 +2773,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>176</v>
       </c>
@@ -2756,7 +2784,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>179</v>
       </c>
@@ -2767,7 +2795,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>182</v>
       </c>
@@ -2778,7 +2806,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>184</v>
       </c>
@@ -2789,7 +2817,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>186</v>
       </c>
@@ -2800,7 +2828,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>188</v>
       </c>
@@ -2808,7 +2836,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>189</v>
       </c>
@@ -2816,7 +2844,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>190</v>
       </c>
@@ -2824,7 +2852,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>191</v>
       </c>
@@ -2835,7 +2863,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>193</v>
       </c>
@@ -2843,7 +2871,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>194</v>
       </c>
@@ -2851,7 +2879,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>195</v>
       </c>
@@ -2859,7 +2887,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>196</v>
       </c>
@@ -2867,12 +2895,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="30">
+    <row r="65" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>198</v>
       </c>
@@ -2883,12 +2911,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="90">
+    <row r="68" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>202</v>
       </c>
@@ -2911,14 +2939,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -2926,7 +2954,7 @@
     <col min="4" max="4" width="59.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2937,12 +2965,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>206</v>
       </c>
@@ -2953,7 +2981,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>209</v>
       </c>
@@ -2964,7 +2992,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>212</v>
       </c>
@@ -2975,7 +3003,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>215</v>
       </c>
@@ -2986,7 +3014,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>218</v>
       </c>
@@ -3009,14 +3037,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -3024,7 +3052,7 @@
     <col min="4" max="4" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3035,14 +3063,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>221</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>222</v>
       </c>
@@ -3053,7 +3081,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>225</v>
       </c>
@@ -3076,14 +3104,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -3091,7 +3119,7 @@
     <col min="4" max="4" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3102,14 +3130,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>228</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>227</v>
       </c>
@@ -3120,7 +3148,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>231</v>
       </c>
@@ -3143,14 +3171,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -3158,7 +3186,7 @@
     <col min="4" max="4" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3169,14 +3197,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>234</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>235</v>
       </c>
@@ -3187,7 +3215,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>238</v>
       </c>

</xml_diff>

<commit_message>
Changing vignette to use ggflow instead of pplot
</commit_message>
<xml_diff>
--- a/vignettes/table_of_functions.xlsx
+++ b/vignettes/table_of_functions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogers/git/R/packages/wadeTools/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B475E8-C1B0-D84D-BEEF-235E6A053857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCC96F3-EEB0-0346-B46B-6E0C1CBA9B32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="879" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -951,10 +951,10 @@
     <t>**ggflow**</t>
   </si>
   <si>
-    <t>Draw a FlowJo-style (sort of) Plot (DEPRECATED)</t>
-  </si>
-  <si>
     <t>Draw a FlowJo-style (sort of) Plot (much more powerful version of pplot)</t>
+  </si>
+  <si>
+    <t>Draw a FlowJo-style (sort of) Plot (**DEPRECATED**)</t>
   </si>
 </sst>
 </file>
@@ -1743,7 +1743,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1885,7 +1885,7 @@
         <v>294</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1893,7 +1893,7 @@
         <v>304</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>